<commit_message>
File changed with adding errors
</commit_message>
<xml_diff>
--- a/5. Machine Learning/Student_Data.xlsx
+++ b/5. Machine Learning/Student_Data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FD305E-EBFD-44DA-B243-622A4F68CB59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C113A3-5277-441A-8E9A-9B2BA0F5FCBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Mihir</t>
   </si>
   <si>
-    <t>Avg. Marks</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Good </t>
+  </si>
+  <si>
+    <t>Total Marks</t>
   </si>
 </sst>
 </file>
@@ -400,12 +400,13 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -416,10 +417,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -430,10 +431,11 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>89</v>
+        <f>89*12</f>
+        <v>1068</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -444,10 +446,11 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>88</v>
+        <f>88*12</f>
+        <v>1056</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -458,10 +461,11 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>87.5</v>
+        <f>88*12</f>
+        <v>1056</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -471,12 +475,6 @@
       <c r="B5">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>85</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -486,24 +484,23 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>85</v>
+        <f>84*12</f>
+        <v>1008</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>12</v>
-      </c>
       <c r="C7">
-        <v>84</v>
+        <f>79*12</f>
+        <v>948</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -514,10 +511,11 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>79</v>
+        <f>78*12</f>
+        <v>936</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -528,10 +526,11 @@
         <v>17</v>
       </c>
       <c r="C9">
-        <v>78.5</v>
+        <f>76*12</f>
+        <v>912</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -542,10 +541,11 @@
         <v>18</v>
       </c>
       <c r="C10">
-        <v>78</v>
+        <f>74*12</f>
+        <v>888</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -556,10 +556,11 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>78</v>
+        <f>72*12</f>
+        <v>864</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>